<commit_message>
price, ifexist route added
</commit_message>
<xml_diff>
--- a/documentation/routes.xlsx
+++ b/documentation/routes.xlsx
@@ -33,9 +33,10 @@
             <rFont val="Segoe UI"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">GET price of BTC/USD, update every 10 seconds
+          <t>#GET price of BTC/USD, update every 10 seconds
 http://localhost:3000/p?from=BTC&amp;to=USD
-</t>
+#reponses:
+200, 500, 404</t>
         </r>
       </text>
     </comment>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -89,6 +90,15 @@
   </si>
   <si>
     <t>/p</t>
+  </si>
+  <si>
+    <t>/t</t>
+  </si>
+  <si>
+    <t>ticker</t>
+  </si>
+  <si>
+    <t>return basic info of a currency</t>
   </si>
 </sst>
 </file>
@@ -147,16 +157,16 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -178,8 +188,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D5285AC8-B548-4942-B913-21385F26373D}" name="Tabelle1" displayName="Tabelle1" ref="A3:E6" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
-  <autoFilter ref="A3:E6" xr:uid="{8CEDB9FA-36EA-4FC8-9CB3-16C89C35E2E5}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D5285AC8-B548-4942-B913-21385F26373D}" name="Tabelle1" displayName="Tabelle1" ref="A3:E7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A3:E7" xr:uid="{8CEDB9FA-36EA-4FC8-9CB3-16C89C35E2E5}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -187,11 +197,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B07374CE-828A-4D82-BC73-B5A0BF96A33A}" name="No." dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{17E95518-3512-4F51-BED1-AAD514B18DCF}" name="Route" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{35AD3B42-7959-4CEE-8330-57D19CF02767}" name="Name" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{B9289F4D-6CF9-4EFD-BA37-E832D5DFE4A1}" name="Method" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{79D71783-90AB-4415-AC06-5B9014FD7BE3}" name="Description" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{B07374CE-828A-4D82-BC73-B5A0BF96A33A}" name="No." dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{17E95518-3512-4F51-BED1-AAD514B18DCF}" name="Route" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{35AD3B42-7959-4CEE-8330-57D19CF02767}" name="Name" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{B9289F4D-6CF9-4EFD-BA37-E832D5DFE4A1}" name="Method" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{79D71783-90AB-4415-AC06-5B9014FD7BE3}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -460,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:E6"/>
+  <dimension ref="A3:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,6 +553,23 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
updated /ind && compiled tulind
</commit_message>
<xml_diff>
--- a/documentation/routes.xlsx
+++ b/documentation/routes.xlsx
@@ -196,9 +196,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>params</t>
-  </si>
-  <si>
     <t>pair</t>
   </si>
   <si>
@@ -229,9 +226,6 @@
     <t xml:space="preserve">the symbol to be checked </t>
   </si>
   <si>
-    <t>http://localhost:8080/ind?type=rsi&amp;params=14&amp;pair=BTC,USD&amp;timeframe=1440</t>
-  </si>
-  <si>
     <t>http://localhost:8080/if/BTC</t>
   </si>
   <si>
@@ -242,6 +236,12 @@
   </si>
   <si>
     <t>( status in indicators.xlsx)</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/ind?type=rsi&amp;options=14&amp;pair=BTC,USD&amp;timeframe=1440</t>
   </si>
 </sst>
 </file>
@@ -1478,7 +1478,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18">
@@ -1496,22 +1496,22 @@
     </row>
     <row r="14" spans="2:4">
       <c r="C14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="C15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1575,7 +1575,7 @@
         <v>36</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="18">
@@ -1583,7 +1583,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18">
@@ -1615,7 +1615,7 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -1663,28 +1663,28 @@
     </row>
     <row r="7" spans="2:4" ht="15.6">
       <c r="B7" s="15" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="15"/>
     </row>
     <row r="8" spans="2:4" ht="15.6">
       <c r="B8" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="15"/>
     </row>
     <row r="9" spans="2:4" ht="15.6">
       <c r="B9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>42</v>
       </c>
       <c r="D9" s="15"/>
     </row>
@@ -1698,7 +1698,7 @@
         <v>28</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="18">
@@ -1706,12 +1706,12 @@
         <v>30</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="C14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
able to call data from crypto compare
</commit_message>
<xml_diff>
--- a/documentation/routes.xlsx
+++ b/documentation/routes.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593DED82-77A6-4D62-986D-B5AA0B13BE28}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -241,7 +242,7 @@
     <t>options</t>
   </si>
   <si>
-    <t>http://localhost:8080/ind?type=rsi&amp;options=14&amp;pair=BTC,USD&amp;timeframe=1440</t>
+    <t>http://localhost:8080/ind?type=sma&amp;options=14&amp;pair=BTC,USD&amp;timeframe=60</t>
   </si>
 </sst>
 </file>
@@ -1615,7 +1616,7 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
ind route: updated timeframe format
</commit_message>
<xml_diff>
--- a/documentation/routes.xlsx
+++ b/documentation/routes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593DED82-77A6-4D62-986D-B5AA0B13BE28}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574DFA2B-A552-48BF-8037-D5FC40C8371B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -203,9 +203,6 @@
     <t>timeframe</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>array of 0-4 intergers</t>
   </si>
   <si>
@@ -242,7 +239,10 @@
     <t>options</t>
   </si>
   <si>
-    <t>http://localhost:8080/ind?type=sma&amp;options=14&amp;pair=BTC,USD&amp;timeframe=60</t>
+    <t>Currently supported: H1</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/ind?type=sma&amp;options=10&amp;pair=BTC,USD&amp;timeframe=H1</t>
   </si>
 </sst>
 </file>
@@ -1479,7 +1479,7 @@
         <v>28</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18">
@@ -1497,22 +1497,22 @@
     </row>
     <row r="14" spans="2:4">
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="C15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="C16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1576,7 +1576,7 @@
         <v>36</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="18">
@@ -1584,7 +1584,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18">
@@ -1664,10 +1664,10 @@
     </row>
     <row r="7" spans="2:4" ht="15.6">
       <c r="B7" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="15"/>
     </row>
@@ -1676,7 +1676,7 @@
         <v>39</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="15"/>
     </row>
@@ -1685,9 +1685,11 @@
         <v>40</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="2:4" ht="15.6">
       <c r="B10" s="15"/>
@@ -1707,12 +1709,12 @@
         <v>30</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>